<commit_message>
add gitignore and cleanup
</commit_message>
<xml_diff>
--- a/printer_counters.xlsx
+++ b/printer_counters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
   </bookViews>
   <sheets>
-    <sheet name="2026.01" sheetId="2" r:id="rId1"/>
-    <sheet name="2026.02" sheetId="1" r:id="rId2"/>
+    <sheet sheetId="2" name="2026.01" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="2026.02" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -66,41 +66,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <charset val="129"/>
+      <family val="3"/>
       <sz val="11"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,7 +125,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,20 +403,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="12" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>44992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>36734</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>28166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>112802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>20786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>50339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>73692</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>201319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>279135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5">
+        <v>8973</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>23110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>57792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5">
+        <v>156475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>8596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>10301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
+        <v>44538</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>61566</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>42634</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" ht="16.5" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -456,7 +698,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -474,7 +716,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -492,7 +734,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -510,7 +752,7 @@
         <v>4795</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -528,7 +770,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -546,7 +788,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -564,7 +806,7 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -582,7 +824,7 @@
         <v>2657</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -600,7 +842,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -618,7 +860,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -636,7 +878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -654,7 +896,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -672,7 +914,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -690,7 +932,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -708,7 +950,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -726,7 +968,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -744,7 +986,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -762,7 +1004,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -780,7 +1022,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" ht="16.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -799,261 +1041,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C2:C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="12" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>44884</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5">
-        <v>36703</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
-        <v>28137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5">
-        <v>112449</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>4176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5">
-        <v>20608</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
-        <v>50278</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5">
-        <v>73572</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5">
-        <v>201319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5">
-        <v>279133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5">
-        <v>8973</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="5">
-        <v>23105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5">
-        <v>57668</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5">
-        <v>156293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5">
-        <v>8594</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="5">
-        <v>10279</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5">
-        <v>44520</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="5">
-        <v>61551</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5">
-        <v>45141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5">
-        <v>42547</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
-</worksheet>
 </file>
</xml_diff>